<commit_message>
25 nisan pazartesi yedeklemesi
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9D6B99-0665-48DE-B6D4-1C1FCEB4580A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25699C48-05A3-420C-95AA-2D12330BEE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="15468" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\Output\</t>
+  </si>
+  <si>
+    <t>GELİŞTİRME BU DEPO YERİ ÜZERİNDEN YAPILDI.</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -745,6 +748,9 @@
       </c>
       <c r="B15" s="8">
         <v>3001</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
tek depoyerli son revizyon. revizyon tarihi: 26.04.2022
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25699C48-05A3-420C-95AA-2D12330BEE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23DBF7F-F9A9-4495-9750-1BEEFA7684E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="15468" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -245,7 +245,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +255,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -287,6 +299,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -606,7 +624,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -697,19 +715,19 @@
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="10" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="6"/>
@@ -743,46 +761,46 @@
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
+      <c r="A15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="8">
-        <v>3001</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B15" s="12">
+        <v>3002</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="8">
-        <v>3002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="8">
-        <v>3003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="8">
-        <v>3004</v>
-      </c>
-    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="8">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="8">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="8">
+        <v>3004</v>
+      </c>
+    </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
revize max list length
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23DBF7F-F9A9-4495-9750-1BEEFA7684E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11889D77-CCD8-4470-9D5D-0F020090B70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="12">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
tutarsal öncesi son yedekleme
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11889D77-CCD8-4470-9D5D-0F020090B70C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915393BC-A66D-48CC-B8D7-2E7774D4D317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="12">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
DÖKÜM YAPMADAN ÖNCE SON YEDEKLEME
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915393BC-A66D-48CC-B8D7-2E7774D4D317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21D9E65-AFE6-41FC-A795-4EDF3BE274BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="12">
-        <v>3002</v>
+        <v>3003</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
döküm çalışması öncesi son yedekleme
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21D9E65-AFE6-41FC-A795-4EDF3BE274BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50621EBB-C1E0-44C9-9FFF-EE4AFF4FB089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
         <v>53</v>
       </c>
       <c r="B15" s="12">
-        <v>3003</v>
+        <v>3001</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Dosya yoluna sırlama adı yazıldı
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\can.sarihan\Documents\UiPath\RPA_Cogi_Sirlama_REF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50621EBB-C1E0-44C9-9FFF-EE4AFF4FB089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41ACF1F-0A0C-4BAB-B7B9-78D40A6AF830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -201,26 +201,29 @@
     <t>DepoYeri_1</t>
   </si>
   <si>
-    <t>DepoYeri_2</t>
-  </si>
-  <si>
-    <t>DepoYeri_3</t>
-  </si>
-  <si>
-    <t>DepoYeri_4</t>
-  </si>
-  <si>
-    <t>C:\Users\can.sarihan\Documents\UiPath\COGİ_Otomasyonu_REF\Data\Output\</t>
-  </si>
-  <si>
-    <t>GELİŞTİRME BU DEPO YERİ ÜZERİNDEN YAPILDI.</t>
+    <t>OTOMASYON YÖNETİM ALANI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP KULLANICI </t>
+  </si>
+  <si>
+    <t>SAP ŞİFRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÇIKTI RAPORUN DOSYA KONUMU </t>
+  </si>
+  <si>
+    <t>SAP EKRANINA YAZILAN DEPO YERİ</t>
+  </si>
+  <si>
+    <t>C:\Users\can.sarihan\Documents\UiPath\RPA_Cogi_Sirlama_REF\Data\Output\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,8 +247,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,18 +278,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -279,11 +291,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -294,19 +321,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +649,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -710,105 +735,98 @@
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="9">
         <v>3001</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="8">
-        <v>3002</v>
-      </c>
+    <row r="17" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="18" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="8">
-        <v>3003</v>
-      </c>
+    <row r="23" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A24" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="8">
-        <v>3004</v>
-      </c>
+    <row r="24" spans="2:2" ht="14.25" customHeight="1">
+      <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="2:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="2:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1777,6 +1795,9 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:C8"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>